<commit_message>
Create shoe database entries
</commit_message>
<xml_diff>
--- a/Shoe.xlsx
+++ b/Shoe.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Shoe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="23040" windowHeight="9383"/>
   </bookViews>
   <sheets>
     <sheet name="Weartesters" sheetId="1" r:id="rId1"/>
@@ -432,15 +432,16 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1"/>
+    <col min="2" max="6" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -466,7 +467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +493,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -518,7 +519,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -544,7 +545,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -570,7 +571,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -596,7 +597,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -622,7 +623,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -648,7 +649,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -674,7 +675,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -700,7 +701,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -726,7 +727,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -752,7 +753,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -778,7 +779,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -804,7 +805,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -830,7 +831,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -856,7 +857,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>